<commit_message>
Ajusta: implementação e saídas
- Muda a saída e a quantidade de arquivos de saída
- Altera nome dos arquivos dos notebooks
- Adiciona arquivos com as melhores métricas na pasta de Avaliações
</commit_message>
<xml_diff>
--- a/Random Forest Regressor/plot_infos_RFR_msc.xlsx
+++ b/Random Forest Regressor/plot_infos_RFR_msc.xlsx
@@ -500,7 +500,7 @@
         <v>0.9528879599269071</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9796781031583103</v>
+        <v>0.9796781031583108</v>
       </c>
       <c r="E2" t="n">
         <v>0.5765787952594664</v>
@@ -518,7 +518,7 @@
         <v>1.092269736159219</v>
       </c>
       <c r="J2" t="n">
-        <v>-1.307832170883536</v>
+        <v>-1.30783217088354</v>
       </c>
     </row>
     <row r="3">
@@ -536,7 +536,7 @@
         <v>0.6693137744219941</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8181214572302192</v>
+        <v>0.8181214572302193</v>
       </c>
       <c r="E3" t="n">
         <v>1.527568744069197</v>
@@ -572,7 +572,7 @@
         <v>0.6593301616705328</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8152092733598374</v>
+        <v>0.8152092733598373</v>
       </c>
       <c r="E4" t="n">
         <v>1.228235463649648</v>
@@ -587,10 +587,10 @@
         <v>58.36692884926079</v>
       </c>
       <c r="I4" t="n">
-        <v>0.918680897222842</v>
+        <v>0.9186808972228417</v>
       </c>
       <c r="J4" t="n">
-        <v>1.126119374926654</v>
+        <v>1.126119374926658</v>
       </c>
     </row>
     <row r="5">
@@ -608,7 +608,7 @@
         <v>0.9119615818991345</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9671286736826724</v>
+        <v>0.9671286736826732</v>
       </c>
       <c r="E5" t="n">
         <v>0.1739987787903575</v>
@@ -644,7 +644,7 @@
         <v>0.4484747780817208</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6704804706365269</v>
+        <v>0.6704804706365277</v>
       </c>
       <c r="E6" t="n">
         <v>0.4355046274991969</v>
@@ -680,7 +680,7 @@
         <v>0.5411032598703787</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7491148305023667</v>
+        <v>0.7491148305023666</v>
       </c>
       <c r="E7" t="n">
         <v>0.2962905714412796</v>
@@ -716,7 +716,7 @@
         <v>0.9073918543949527</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9710628656121723</v>
+        <v>0.9710628656121727</v>
       </c>
       <c r="E8" t="n">
         <v>0.0938572761088423</v>
@@ -752,7 +752,7 @@
         <v>0.3221603163762145</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5692949280815077</v>
+        <v>0.5692949280815075</v>
       </c>
       <c r="E9" t="n">
         <v>0.2539258105973082</v>
@@ -767,10 +767,10 @@
         <v>82.33101989066974</v>
       </c>
       <c r="I9" t="n">
-        <v>0.9510970920905539</v>
+        <v>0.9510970920905537</v>
       </c>
       <c r="J9" t="n">
-        <v>0.1509844328975136</v>
+        <v>0.1509844328975145</v>
       </c>
     </row>
     <row r="10">
@@ -824,7 +824,7 @@
         <v>0.9205075361857782</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9694159256430205</v>
+        <v>0.9694159256430215</v>
       </c>
       <c r="E11" t="n">
         <v>28.97539575321897</v>
@@ -896,7 +896,7 @@
         <v>0.476628784031723</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7203147900447806</v>
+        <v>0.7203147900447805</v>
       </c>
       <c r="E13" t="n">
         <v>55.89000164843432</v>
@@ -932,7 +932,7 @@
         <v>0.9364021347367469</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9742698963355337</v>
+        <v>0.9742698963355333</v>
       </c>
       <c r="E14" t="n">
         <v>0.8112396202693049</v>
@@ -968,7 +968,7 @@
         <v>0.593532061265899</v>
       </c>
       <c r="D15" t="n">
-        <v>0.7705149490875671</v>
+        <v>0.770514949087567</v>
       </c>
       <c r="E15" t="n">
         <v>2.050883690973463</v>
@@ -1004,7 +1004,7 @@
         <v>0.6284948492907074</v>
       </c>
       <c r="D16" t="n">
-        <v>0.8344531007954668</v>
+        <v>0.8344531007954665</v>
       </c>
       <c r="E16" t="n">
         <v>1.320872749367568</v>
@@ -1019,10 +1019,10 @@
         <v>60.95122235930077</v>
       </c>
       <c r="I16" t="n">
-        <v>0.7650965480388</v>
+        <v>0.7650965480388002</v>
       </c>
       <c r="J16" t="n">
-        <v>3.493593198615249</v>
+        <v>3.493593198615246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>